<commit_message>
Ajout formulaire de renseignement HSE
</commit_message>
<xml_diff>
--- a/#AUTRES/Formulaires De Renseignement/genius-formulaire-de-renseignement-dut-gea-aix-grh.xlsx
+++ b/#AUTRES/Formulaires De Renseignement/genius-formulaire-de-renseignement-dut-gea-aix-grh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOUVEAU\Desktop\Genius\#AUTRES\Formulaires De Renseignement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7F6A43-5BAA-45FC-9831-8624F12BA703}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22586D8-8682-41DB-8CE7-DFC365AEC6EA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,6 +693,7 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -702,7 +703,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2032,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2768,11 +2768,11 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="28">
+      <c r="A41" s="25">
         <f>D21</f>
         <v>2</v>
       </c>
-      <c r="B41" s="28">
+      <c r="B41" s="25">
         <f>D22</f>
         <v>3</v>
       </c>
@@ -2782,7 +2782,7 @@
       <c r="D41" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="25"/>
+      <c r="E41" s="26"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2790,11 +2790,11 @@
       <c r="J41" s="3"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="28">
+      <c r="A42" s="25">
         <f>D21</f>
         <v>2</v>
       </c>
-      <c r="B42" s="28">
+      <c r="B42" s="25">
         <f>D23</f>
         <v>4</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="D42" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="26"/>
+      <c r="E42" s="27"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -2812,11 +2812,11 @@
       <c r="J42" s="3"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28">
+      <c r="A43" s="25">
         <f>D21</f>
         <v>2</v>
       </c>
-      <c r="B43" s="28">
+      <c r="B43" s="25">
         <f>D24</f>
         <v>5</v>
       </c>
@@ -2826,7 +2826,7 @@
       <c r="D43" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="26"/>
+      <c r="E43" s="27"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2834,11 +2834,11 @@
       <c r="J43" s="3"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="28">
+      <c r="A44" s="25">
         <f>D21</f>
         <v>2</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="25">
         <f>D25</f>
         <v>6</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="D44" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E44" s="26"/>
+      <c r="E44" s="27"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2856,11 +2856,11 @@
       <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="28">
+      <c r="A45" s="25">
         <f>D22</f>
         <v>3</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="25">
         <f>D23</f>
         <v>4</v>
       </c>
@@ -2870,7 +2870,7 @@
       <c r="D45" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="27"/>
+      <c r="E45" s="28"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -2878,11 +2878,11 @@
       <c r="J45" s="3"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="28">
+      <c r="A46" s="25">
         <f>D22</f>
         <v>3</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="25">
         <f>D24</f>
         <v>5</v>
       </c>
@@ -2896,11 +2896,11 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="28">
+      <c r="A47" s="25">
         <f>D22</f>
         <v>3</v>
       </c>
-      <c r="B47" s="28">
+      <c r="B47" s="25">
         <f>D25</f>
         <v>6</v>
       </c>
@@ -2914,11 +2914,11 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28">
+      <c r="A48" s="25">
         <f>D23</f>
         <v>4</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B48" s="25">
         <f>D24</f>
         <v>5</v>
       </c>
@@ -2932,11 +2932,11 @@
       <c r="J48" s="3"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="28">
+      <c r="A49" s="25">
         <f>D23</f>
         <v>4</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B49" s="25">
         <f>D25</f>
         <v>6</v>
       </c>
@@ -2950,11 +2950,11 @@
       <c r="J49" s="3"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="28">
+      <c r="A50" s="25">
         <f>D24</f>
         <v>5</v>
       </c>
-      <c r="B50" s="28">
+      <c r="B50" s="25">
         <f>D25</f>
         <v>6</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>114</v>
       </c>
       <c r="B106" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D41,""");")</f>
+        <f t="shared" ref="B106:B115" si="4">CONCATENATE("INSERT INTO job (JobName) VALUES (""",D41,""");")</f>
         <v>INSERT INTO job (JobName) VALUES ("Responsable de la formation");</v>
       </c>
       <c r="C106" s="3"/>
@@ -3776,7 +3776,7 @@
     <row r="107" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="22"/>
       <c r="B107" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D42,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("Chargé de communication interne");</v>
       </c>
       <c r="C107" s="3"/>
@@ -3791,7 +3791,7 @@
     <row r="108" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="22"/>
       <c r="B108" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D43,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("Responsable rémunérations et avantages sociaux");</v>
       </c>
       <c r="C108" s="3"/>
@@ -3806,7 +3806,7 @@
     <row r="109" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="22"/>
       <c r="B109" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D44,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("Responsable diversité et Responsabilité Sociale et Ethique");</v>
       </c>
       <c r="C109" s="3"/>
@@ -3821,7 +3821,7 @@
     <row r="110" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="22"/>
       <c r="B110" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D45,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("Responsable du recrutement");</v>
       </c>
       <c r="C110" s="3"/>
@@ -3836,7 +3836,7 @@
     <row r="111" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="22"/>
       <c r="B111" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D46,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("");</v>
       </c>
       <c r="C111" s="3" t="str">
@@ -3854,7 +3854,7 @@
     <row r="112" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="22"/>
       <c r="B112" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D47,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("");</v>
       </c>
       <c r="C112" s="3"/>
@@ -3869,7 +3869,7 @@
     <row r="113" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="22"/>
       <c r="B113" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D48,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("");</v>
       </c>
       <c r="C113" s="3"/>
@@ -3884,7 +3884,7 @@
     <row r="114" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="22"/>
       <c r="B114" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D49,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("");</v>
       </c>
       <c r="C114" s="3"/>
@@ -3899,7 +3899,7 @@
     <row r="115" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="22"/>
       <c r="B115" s="23" t="str">
-        <f>CONCATENATE("INSERT INTO job (JobName) VALUES (""",D50,""");")</f>
+        <f t="shared" si="4"/>
         <v>INSERT INTO job (JobName) VALUES ("");</v>
       </c>
       <c r="C115" s="3"/>
@@ -4057,7 +4057,7 @@
     <row r="126" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="22"/>
       <c r="B126" s="23" t="str">
-        <f t="shared" ref="B126:B134" si="4">CONCATENATE("INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);")</f>
+        <f t="shared" ref="B126:B134" si="5">CONCATENATE("INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);")</f>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C126" s="3"/>
@@ -4074,7 +4074,7 @@
     <row r="127" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="22"/>
       <c r="B127" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C127" s="3"/>
@@ -4089,7 +4089,7 @@
     <row r="128" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="22"/>
       <c r="B128" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C128" s="3"/>
@@ -4104,7 +4104,7 @@
     <row r="129" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="22"/>
       <c r="B129" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C129" s="3"/>
@@ -4119,7 +4119,7 @@
     <row r="130" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="22"/>
       <c r="B130" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C130" s="3"/>
@@ -4134,7 +4134,7 @@
     <row r="131" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="22"/>
       <c r="B131" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C131" s="3"/>
@@ -4149,7 +4149,7 @@
     <row r="132" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="22"/>
       <c r="B132" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C132" s="3"/>
@@ -4164,7 +4164,7 @@
     <row r="133" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="22"/>
       <c r="B133" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C133" s="3"/>
@@ -4179,7 +4179,7 @@
     <row r="134" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="22"/>
       <c r="B134" s="23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,2);</v>
       </c>
       <c r="C134" s="3"/>
@@ -4221,7 +4221,7 @@
     <row r="137" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="22"/>
       <c r="B137" s="23" t="str">
-        <f t="shared" ref="B137:B140" si="5">CONCATENATE("INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,3);")</f>
+        <f t="shared" ref="B137:B140" si="6">CONCATENATE("INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,3);")</f>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,3);</v>
       </c>
       <c r="C137" s="3"/>
@@ -4236,7 +4236,7 @@
     <row r="138" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="22"/>
       <c r="B138" s="23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,3);</v>
       </c>
       <c r="C138" s="3"/>
@@ -4251,7 +4251,7 @@
     <row r="139" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="22"/>
       <c r="B139" s="23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,3);</v>
       </c>
       <c r="C139" s="3"/>
@@ -4266,7 +4266,7 @@
     <row r="140" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="22"/>
       <c r="B140" s="23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO association_job_skill (IDJob, IDSkill, IDRank) VALUES (1,1,3);</v>
       </c>
       <c r="C140" s="3"/>

</xml_diff>